<commit_message>
Automatische test-sync: 2025-08-28 17:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,8 +725,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-28 17:37:41</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -746,7 +788,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -754,17 +796,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -806,7 +848,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 17:50:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,8 +767,50 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-28 17:50:25</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -788,7 +830,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -796,17 +838,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -848,7 +890,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,8 +809,92 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:04:08</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:04:08</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -830,7 +914,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -838,17 +922,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -890,7 +974,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,8 +893,50 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:05:29</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -914,7 +956,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -922,17 +964,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -974,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,8 +935,50 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:15:13</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -956,7 +998,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -964,17 +1006,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1016,7 +1058,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -977,8 +977,50 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:16:14</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -998,7 +1040,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1006,17 +1048,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1058,7 +1100,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1019,8 +1019,50 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:37:11</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1040,7 +1082,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1048,17 +1090,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1100,7 +1142,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 18:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,8 +1061,50 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-28 18:38:08</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1082,7 +1124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1090,17 +1132,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1184,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,8 +1103,50 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:11:08</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1124,7 +1166,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1132,17 +1174,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1184,7 +1226,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,8 +1145,50 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:21:11</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1166,7 +1208,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1174,17 +1216,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1226,7 +1268,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,8 +1187,50 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:34:02</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1208,7 +1250,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1216,17 +1258,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1268,7 +1310,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1229,8 +1229,50 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:35:36</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1250,7 +1292,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1258,17 +1300,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1310,7 +1352,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1271,8 +1271,50 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:37:22</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1292,7 +1334,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1300,17 +1342,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1352,7 +1394,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 20:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,8 +1313,50 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Kan je dit bestellen?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;inkoop@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-28 20:56:03</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1334,7 +1376,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1342,17 +1384,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1367,7 +1409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1397,6 +1439,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1355,8 +1355,50 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:01:03</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1376,7 +1418,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1384,17 +1426,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1436,7 +1478,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1397,8 +1397,50 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Retour status</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:02:06</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1418,7 +1460,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1426,17 +1468,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1478,7 +1520,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,8 +1439,50 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Opvolging retour</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:05:09</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1460,7 +1502,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1468,17 +1510,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1520,7 +1562,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,8 +1481,50 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Nieuwe bestelling</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:06:14</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1502,7 +1544,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1510,17 +1552,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1572,7 +1614,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1523,8 +1523,50 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Opvolging bestelling</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:08:16</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1544,7 +1586,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1552,17 +1594,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1577,7 +1619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1617,6 +1659,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1565,8 +1565,50 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Afspraak demo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:10:20</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1586,7 +1628,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1594,17 +1636,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1619,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1669,6 +1711,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1607,8 +1607,50 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Opvolging afspraak</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:12:24</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1628,7 +1670,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1636,17 +1678,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1704,17 +1746,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1649,8 +1649,50 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CE-certificaat aanvraag</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:14:27</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1670,7 +1712,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1678,17 +1720,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1703,7 +1745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1763,6 +1805,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1691,8 +1691,50 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Opvolging certificaat</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:16:30</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1712,7 +1754,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1720,17 +1762,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1798,17 +1840,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Kwaliteit / Certificaten</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kwaliteit / Certificaten</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1733,8 +1733,50 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Klacht levering</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:18:34</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1754,7 +1796,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1762,17 +1804,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1787,7 +1829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1857,6 +1899,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1775,8 +1775,50 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Opvolging klacht</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:20:37</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1796,7 +1838,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1804,17 +1846,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1892,17 +1934,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1817,8 +1817,50 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Datasheet verzoek</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:22:41</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1838,7 +1880,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1846,17 +1888,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1871,7 +1913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1924,7 +1966,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kwaliteit / Certificaten</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1934,7 +1976,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Kwaliteit / Certificaten</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1948,6 +1990,16 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1859,8 +1859,50 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Opvolging datasheet</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:24:45</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1880,7 +1922,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1888,17 +1930,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1986,17 +2028,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:27:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1901,8 +1901,50 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bel klant</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:26:51</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1922,7 +1964,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1930,17 +1972,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="J2:J31">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1955,7 +1997,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2008,7 +2050,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Kwaliteit / Certificaten</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2018,7 +2060,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kwaliteit / Certificaten</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2028,7 +2070,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2042,6 +2084,16 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-28 21:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-28.xlsx
+++ b/logs/mail_log_2025-08-28.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1943,8 +1943,50 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Opvolging contact</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-08-28 21:28:55</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1964,7 +2006,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1972,17 +2014,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
+  <conditionalFormatting sqref="H2:H32">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I31">
+  <conditionalFormatting sqref="I2:I32">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J31">
+  <conditionalFormatting sqref="J2:J32">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2040,7 +2082,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2050,7 +2092,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kwaliteit / Certificaten</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2060,7 +2102,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Kwaliteit / Certificaten</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2080,11 +2122,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">

</xml_diff>